<commit_message>
Added Jan 28 Tournament
</commit_message>
<xml_diff>
--- a/exports/d_elo_time_table.xlsx
+++ b/exports/d_elo_time_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1300,6 +1300,202 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr"/>
     </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>-17.40927553185213</v>
+      </c>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="n">
+        <v>17.40927553185213</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" t="n">
+        <v>6.146545249736358</v>
+      </c>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>-6.146545249736356</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" t="n">
+        <v>-23.03791779652222</v>
+      </c>
+      <c r="C64" t="n">
+        <v>23.03791779652222</v>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="n">
+        <v>-10.95195006581875</v>
+      </c>
+      <c r="F65" t="n">
+        <v>10.95195006581875</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="n">
+        <v>9.327181778093486</v>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
+        <v>-9.327181778093484</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="n">
+        <v>11.3121180763797</v>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="n">
+        <v>-11.3121180763797</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="n">
+        <v>-17.23351129782776</v>
+      </c>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>17.23351129782776</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="n">
+        <v>5.095205994447398</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>-5.095205994447396</v>
+      </c>
+      <c r="F69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="n">
+        <v>9.456519108265985</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-9.456519108265981</v>
+      </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="n">
+        <v>-7.924851840315794</v>
+      </c>
+      <c r="F71" t="n">
+        <v>7.924851840315796</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="n">
+        <v>8.974044534140853</v>
+      </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>-8.974044534140855</v>
+      </c>
+      <c r="F72" t="inlineStr"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="n">
+        <v>-20.61844630140414</v>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="n">
+        <v>20.61844630140414</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-17.2985575863854</v>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="n">
+        <v>17.2985575863854</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-14.36305800477309</v>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="n">
+        <v>14.36305800477309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Gen 9 RU Tourney
</commit_message>
<xml_diff>
--- a/exports/d_elo_time_table.xlsx
+++ b/exports/d_elo_time_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2459,16 +2459,16 @@
         <v>125</v>
       </c>
       <c r="B126" t="inlineStr"/>
-      <c r="C126" t="n">
-        <v>-11.97066741944268</v>
-      </c>
+      <c r="C126" t="inlineStr"/>
       <c r="D126" t="inlineStr"/>
-      <c r="E126" t="n">
-        <v>11.97066741944269</v>
-      </c>
+      <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr"/>
-      <c r="G126" t="inlineStr"/>
-      <c r="H126" t="inlineStr"/>
+      <c r="G126" t="n">
+        <v>-14.91601092197619</v>
+      </c>
+      <c r="H126" t="n">
+        <v>14.91601092197619</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -2477,13 +2477,45 @@
       <c r="B127" t="inlineStr"/>
       <c r="C127" t="inlineStr"/>
       <c r="D127" t="inlineStr"/>
-      <c r="E127" t="n">
-        <v>-18.60015413979376</v>
-      </c>
+      <c r="E127" t="inlineStr"/>
       <c r="F127" t="inlineStr"/>
-      <c r="G127" t="inlineStr"/>
+      <c r="G127" t="n">
+        <v>-12.41739680548837</v>
+      </c>
       <c r="H127" t="n">
-        <v>18.60015413979376</v>
+        <v>12.41739680548837</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="n">
+        <v>-11.97066741944268</v>
+      </c>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="n">
+        <v>11.97066741944269</v>
+      </c>
+      <c r="F128" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="n">
+        <v>-16.31453075323677</v>
+      </c>
+      <c r="F129" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" t="n">
+        <v>16.31453075323677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>